<commit_message>
Draft 4 template done
</commit_message>
<xml_diff>
--- a/Individual Journey (70%)/Feeback.xlsx
+++ b/Individual Journey (70%)/Feeback.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MHodg\Desktop\Industry-Engagement\Individual Journey (70%)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3014\Industry-Engagement\Individual Journey (70%)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421F8A9-0B33-44FB-B3B4-0C58AF85A1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1E8A4C-91B6-4FCF-B64A-00816FAEF7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Portfolio Feedback</t>
   </si>
@@ -76,6 +76,13 @@
   </si>
   <si>
     <t>Fixed, I did not have access to the projects repo at the time, now I do I have created a repo on my new github account and added and linked it</t>
+  </si>
+  <si>
+    <t>Tyler Cheng</t>
+  </si>
+  <si>
+    <t>its good
+however the mobile version seem to be a bit off</t>
   </si>
 </sst>
 </file>
@@ -463,24 +470,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.5546875" customWidth="1"/>
-    <col min="3" max="3" width="2.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="37.44140625" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
-    <col min="8" max="8" width="54.88671875" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="3.140625" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -491,7 +496,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -502,7 +507,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -513,7 +518,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
         <v>0</v>
@@ -525,8 +530,9 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -536,8 +542,9 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -550,9 +557,12 @@
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -567,9 +577,12 @@
       <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="C8" s="6">
         <v>2</v>
@@ -581,9 +594,12 @@
       <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="C9" s="6">
         <v>3</v>
@@ -595,9 +611,12 @@
       <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="C10" s="6">
         <v>4</v>
@@ -609,9 +628,12 @@
       <c r="F10" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="C11" s="6">
         <v>5</v>
@@ -623,9 +645,12 @@
       <c r="F11" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -635,55 +660,93 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="6"/>
       <c r="E13" s="6"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="6"/>
       <c r="E14" s="6"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="C15" s="6"/>
       <c r="E15" s="6"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
       <c r="C16" s="6"/>
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E16" s="6"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="C17" s="6"/>
       <c r="E17" s="6"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="C18" s="6"/>
       <c r="E18" s="6"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E19" s="6"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>